<commit_message>
New tip alignments, linked to sources
</commit_message>
<xml_diff>
--- a/tabular/eve/ecv-refseqs-side-data.xlsx
+++ b/tabular/eve/ecv-refseqs-side-data.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
   <si>
     <t>Circovirus</t>
   </si>
@@ -271,6 +271,24 @@
   </si>
   <si>
     <t>Endogenous circoviral element cress.9-conus consensus sequence</t>
+  </si>
+  <si>
+    <t>REF_ECV_Taenia</t>
+  </si>
+  <si>
+    <t>ecv-circo.14-tinamou-con</t>
+  </si>
+  <si>
+    <t>REF_ECV_Tinamou</t>
+  </si>
+  <si>
+    <t>ecv-cress.10-taenia-con</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element circo.14-tinamou consensus sequence</t>
+  </si>
+  <si>
+    <t>Endogenous circoviral element cress.10-taenia consensus sequence</t>
   </si>
 </sst>
 </file>
@@ -354,7 +372,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="408">
+  <cellStyleXfs count="418">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -554,6 +572,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -770,7 +798,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="408">
+  <cellStyles count="418">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -979,6 +1007,11 @@
     <cellStyle name="Followed Hyperlink" xfId="403" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="405" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="407" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="409" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="411" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="413" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="415" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="417" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1178,6 +1211,11 @@
     <cellStyle name="Hyperlink" xfId="402" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="404" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="406" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="408" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="410" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="412" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="414" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="416" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1515,10 +1553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M24"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D12" sqref="A1:M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -2010,26 +2048,26 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>84</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>43</v>
+        <v>87</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="I13" s="3">
         <v>1</v>
@@ -2049,16 +2087,16 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>10</v>
@@ -2068,7 +2106,7 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
@@ -2088,16 +2126,16 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>10</v>
@@ -2107,7 +2145,7 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15" s="3">
         <v>1</v>
@@ -2127,16 +2165,16 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="3" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>10</v>
@@ -2146,7 +2184,7 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I16" s="3">
         <v>1</v>
@@ -2166,16 +2204,16 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="3" t="s">
-        <v>21</v>
+        <v>77</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>33</v>
+        <v>78</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>10</v>
@@ -2185,7 +2223,7 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I17" s="3">
         <v>1</v>
@@ -2205,16 +2243,16 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>10</v>
@@ -2224,7 +2262,7 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I18" s="3">
         <v>1</v>
@@ -2244,16 +2282,16 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>10</v>
@@ -2263,7 +2301,7 @@
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I19" s="3">
         <v>1</v>
@@ -2283,16 +2321,16 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>10</v>
@@ -2302,7 +2340,7 @@
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I20" s="3">
         <v>1</v>
@@ -2322,26 +2360,26 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="3" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>56</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>6</v>
+      <c r="F21" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="I21" s="3">
         <v>1</v>
@@ -2361,22 +2399,22 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="3" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>81</v>
+      <c r="C22" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>7</v>
+      <c r="F22" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3">
@@ -2399,11 +2437,86 @@
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="B23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3">
+        <v>9</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1</v>
+      </c>
+      <c r="J23" s="3">
+        <v>1</v>
+      </c>
+      <c r="K23" s="3">
+        <v>1</v>
+      </c>
+      <c r="L23" s="3">
+        <v>1</v>
+      </c>
+      <c r="M23" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3">
+        <v>10</v>
+      </c>
+      <c r="I24" s="3">
+        <v>1</v>
+      </c>
+      <c r="J24" s="3">
+        <v>1</v>
+      </c>
+      <c r="K24" s="3">
+        <v>1</v>
+      </c>
+      <c r="L24" s="3">
+        <v>1</v>
+      </c>
+      <c r="M24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
     </row>
   </sheetData>
   <sortState ref="A2:M17">

</xml_diff>